<commit_message>
Merge of estel + martin/javi
</commit_message>
<xml_diff>
--- a/data/gene_ids.xlsx
+++ b/data/gene_ids.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,70 +40,64 @@
     <t xml:space="preserve">pdb</t>
   </si>
   <si>
+    <t xml:space="preserve">myod1_mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myod1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X61655.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7WZ6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ascl1_mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ascl1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q02067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U68534.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ascl1_human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASCL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P50553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG_008950.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">myod1_human</t>
   </si>
   <si>
     <t xml:space="preserve">MYOD1</t>
   </si>
   <si>
-    <t xml:space="preserve">human</t>
-  </si>
-  <si>
     <t xml:space="preserve">P15172</t>
   </si>
   <si>
     <t xml:space="preserve">AF027148.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myod1_mouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myod1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P10085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X61655.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7WZ6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ascl1_human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASCL1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P50553</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG_008950.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ascl1_mouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascl1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q02067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U68534.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
   </si>
 </sst>
 </file>
@@ -203,10 +197,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.49"/>
   </cols>
@@ -259,27 +253,27 @@
         <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>20</v>
@@ -288,27 +282,27 @@
         <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>